<commit_message>
Delete old columns, add new tabs, some fixes and refact
</commit_message>
<xml_diff>
--- a/SNTDataBase/res/1.xlsx
+++ b/SNTDataBase/res/1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CPP_Team\SNTDataBase\SNTDataBase\res\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F857F70-E4AD-4FA2-A0F8-035AF1C1F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="17115" windowHeight="12780"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,10 +31,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="173" formatCode="[$-1010419]dd\.mm\.yyyy"/>
-    <numFmt numFmtId="175" formatCode="[$-1010419]#,##0.00;\-#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$-1010419]dd\.mm\.yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-1010419]#,##0.00;\-#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[$-1010419]#,##0.000;\-#,##0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -66,22 +73,25 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -89,14 +99,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -134,9 +147,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -169,9 +182,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,9 +234,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -379,15 +426,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -407,13 +454,13 @@
       <c r="B1" s="2">
         <v>129</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="4">
         <v>90.933999999999997</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="4">
         <v>78.653000000000006</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="4">
         <v>12.281000000000001</v>
       </c>
     </row>
@@ -424,13 +471,13 @@
       <c r="B2" s="2">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>373.82900000000001</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>177.94800000000001</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>195.881</v>
       </c>
     </row>
@@ -441,13 +488,13 @@
       <c r="B3" s="2">
         <v>79</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>15057.978000000001</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>10272.192000000001</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>4785.7860000000001</v>
       </c>
     </row>
@@ -458,13 +505,13 @@
       <c r="B4" s="2">
         <v>74</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>17172.097000000002</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>8959.0210000000006</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>8117.165</v>
       </c>
     </row>
@@ -475,13 +522,13 @@
       <c r="B5" s="2">
         <v>60</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>17408.079000000002</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>11933.25</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>5474.8289999999997</v>
       </c>
     </row>
@@ -492,13 +539,13 @@
       <c r="B6" s="2">
         <v>32</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>19364.814999999999</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>13404.467000000001</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>5960.348</v>
       </c>
     </row>
@@ -509,13 +556,13 @@
       <c r="B7" s="2">
         <v>41</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>33862.234000000004</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="4">
         <v>22545.885000000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>11316.349</v>
       </c>
     </row>
@@ -526,13 +573,13 @@
       <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>38041.667999999998</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>25660.013999999999</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>12381.654</v>
       </c>
     </row>
@@ -543,13 +590,13 @@
       <c r="B9" s="2">
         <v>54</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>39040.137999999999</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <v>26397.128000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <v>12643.01</v>
       </c>
     </row>
@@ -560,13 +607,13 @@
       <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>10860.19</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <v>8061.89</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>2798.3</v>
       </c>
       <c r="F10" s="3"/>
@@ -580,13 +627,13 @@
       <c r="B11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>142.66</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <v>138.32</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>4.32</v>
       </c>
       <c r="F11" s="3"/>
@@ -600,13 +647,13 @@
       <c r="B12" s="2">
         <v>4</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>9696.27</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="4">
         <v>7725.7300000000005</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>1970.53</v>
       </c>
       <c r="F12" s="3"/>
@@ -620,13 +667,13 @@
       <c r="B13" s="2">
         <v>5</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <v>6263.4000000000005</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="4">
         <v>5165.4400000000005</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>1097.96</v>
       </c>
       <c r="F13" s="3"/>
@@ -640,13 +687,13 @@
       <c r="B14" s="2">
         <v>7</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>1588.81</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="4">
         <v>1236.6100000000001</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <v>352.19</v>
       </c>
       <c r="F14" s="3"/>
@@ -660,13 +707,13 @@
       <c r="B15" s="2">
         <v>8</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>1790.13</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="4">
         <v>1161.1500000000001</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>628.98</v>
       </c>
       <c r="F15" s="3"/>
@@ -680,13 +727,13 @@
       <c r="B16" s="2">
         <v>9</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>1224.6200000000001</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <v>880.76</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>343.85</v>
       </c>
       <c r="F16" s="3"/>
@@ -700,13 +747,13 @@
       <c r="B17" s="2">
         <v>10</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <v>6259.01</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <v>4344.1000000000004</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <v>1914.91</v>
       </c>
       <c r="F17" s="3"/>
@@ -720,13 +767,13 @@
       <c r="B18" s="2">
         <v>11</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
         <v>4103.3999999999996</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="4">
         <v>3168.6</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="4">
         <v>934.79</v>
       </c>
       <c r="F18" s="3"/>
@@ -740,13 +787,13 @@
       <c r="B19" s="2">
         <v>13</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="4">
         <v>3452.63</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="4">
         <v>2961.09</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="4">
         <v>491.54</v>
       </c>
       <c r="F19" s="3"/>
@@ -760,13 +807,13 @@
       <c r="B20" s="2">
         <v>14</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4">
         <v>1083.96</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="4">
         <v>730.19</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="4">
         <v>353.76</v>
       </c>
       <c r="F20" s="3"/>
@@ -780,13 +827,13 @@
       <c r="B21" s="2">
         <v>15</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="4">
         <v>138.28</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <v>118.5</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="4">
         <v>19.78</v>
       </c>
       <c r="F21" s="3"/>
@@ -800,13 +847,13 @@
       <c r="B22" s="2">
         <v>16</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="4">
         <v>1364.98</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="4">
         <v>886.01</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="4">
         <v>478.97</v>
       </c>
       <c r="F22" s="3"/>
@@ -820,13 +867,13 @@
       <c r="B23" s="2">
         <v>18</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="4">
         <v>8918.69</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="4">
         <v>6358.2</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="4">
         <v>2560.4900000000002</v>
       </c>
       <c r="F23" s="3"/>
@@ -840,13 +887,13 @@
       <c r="B24" s="2">
         <v>20</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="4">
         <v>17806</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="4">
         <v>12785.98</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="4">
         <v>5020.01</v>
       </c>
       <c r="F24" s="3"/>
@@ -860,13 +907,13 @@
       <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="4">
         <v>4329.08</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="4">
         <v>2969.53</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="4">
         <v>1359.55</v>
       </c>
       <c r="F25" s="3"/>
@@ -880,13 +927,13 @@
       <c r="B26" s="2">
         <v>22</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="4">
         <v>8901.75</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="4">
         <v>6491.68</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="4">
         <v>2410.06</v>
       </c>
       <c r="F26" s="3"/>
@@ -900,13 +947,13 @@
       <c r="B27" s="2">
         <v>25</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="4">
         <v>26583.22</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="4">
         <v>17562.670000000002</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="4">
         <v>9020.5400000000009</v>
       </c>
       <c r="F27" s="3"/>
@@ -920,13 +967,13 @@
       <c r="B28" s="2">
         <v>26</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="4">
         <v>8305.77</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="4">
         <v>7017.27</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="4">
         <v>1288.5</v>
       </c>
       <c r="F28" s="3"/>
@@ -940,13 +987,13 @@
       <c r="B29" s="2">
         <v>27</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="4">
         <v>2866.73</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="4">
         <v>2606.33</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="4">
         <v>260.39999999999998</v>
       </c>
       <c r="F29" s="3"/>
@@ -960,13 +1007,13 @@
       <c r="B30" s="2">
         <v>28</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="4">
         <v>8402.5499999999993</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="4">
         <v>5708.26</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="4">
         <v>2694.28</v>
       </c>
       <c r="F30" s="3"/>
@@ -980,13 +1027,13 @@
       <c r="B31" s="2">
         <v>29</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="4">
         <v>4117.68</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="4">
         <v>3148.9500000000003</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="4">
         <v>968.72</v>
       </c>
       <c r="F31" s="3"/>
@@ -1000,13 +1047,13 @@
       <c r="B32" s="2">
         <v>30</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="4">
         <v>9876.11</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="4">
         <v>7413.76</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="4">
         <v>2462.34</v>
       </c>
       <c r="F32" s="3"/>
@@ -1020,13 +1067,13 @@
       <c r="B33" s="2">
         <v>31</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="4">
         <v>12.31</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="4">
         <v>4</v>
       </c>
       <c r="F33" s="3"/>
@@ -1040,13 +1087,13 @@
       <c r="B34" s="2">
         <v>33</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="4">
         <v>2329.94</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="4">
         <v>1824.57</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="4">
         <v>505.37</v>
       </c>
       <c r="F34" s="3"/>
@@ -1060,13 +1107,13 @@
       <c r="B35" s="2">
         <v>34</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="4">
         <v>4409.45</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="4">
         <v>3025.31</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="4">
         <v>1384.13</v>
       </c>
       <c r="F35" s="3"/>
@@ -1080,13 +1127,13 @@
       <c r="B36" s="2">
         <v>35</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="4">
         <v>3325.6800000000003</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="4">
         <v>2562.04</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="4">
         <v>763.63</v>
       </c>
       <c r="F36" s="3"/>
@@ -1100,13 +1147,13 @@
       <c r="B37" s="2">
         <v>36</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="4">
         <v>5253.91</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="4">
         <v>3930.88</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="4">
         <v>1323.02</v>
       </c>
       <c r="F37" s="3"/>
@@ -1120,13 +1167,13 @@
       <c r="B38" s="2">
         <v>37</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="4">
         <v>7360.1900000000005</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="4">
         <v>5657.89</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="4">
         <v>1702.3</v>
       </c>
       <c r="F38" s="3"/>
@@ -1140,13 +1187,13 @@
       <c r="B39" s="2">
         <v>39</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="4">
         <v>21877.05</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="4">
         <v>15532.56</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="4">
         <v>6344.4800000000005</v>
       </c>
       <c r="F39" s="3"/>
@@ -1160,13 +1207,13 @@
       <c r="B40" s="2">
         <v>40</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="4">
         <v>5602.39</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="4">
         <v>4311.3100000000004</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="4">
         <v>1291.08</v>
       </c>
       <c r="F40" s="3"/>
@@ -1180,13 +1227,13 @@
       <c r="B41" s="2">
         <v>42</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="4">
         <v>29204.21</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="4">
         <v>17193.25</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="4">
         <v>12010.95</v>
       </c>
       <c r="F41" s="3"/>
@@ -1200,13 +1247,13 @@
       <c r="B42" s="2">
         <v>43</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="4">
         <v>1.04</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="4">
         <v>0.76</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="4">
         <v>0.28000000000000003</v>
       </c>
       <c r="F42" s="3"/>
@@ -1220,13 +1267,13 @@
       <c r="B43" s="2">
         <v>45</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="4">
         <v>12047.42</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="4">
         <v>9271.66</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="4">
         <v>2775.75</v>
       </c>
       <c r="F43" s="3"/>
@@ -1240,13 +1287,13 @@
       <c r="B44" s="2">
         <v>46</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="4">
         <v>1262.55</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="4">
         <v>976.47</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="4">
         <v>286.07</v>
       </c>
       <c r="F44" s="3"/>
@@ -1260,13 +1307,13 @@
       <c r="B45" s="2">
         <v>47</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="4">
         <v>2440.11</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="4">
         <v>2108.92</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="4">
         <v>331.19</v>
       </c>
       <c r="F45" s="3"/>
@@ -1280,13 +1327,13 @@
       <c r="B46" s="2">
         <v>48</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="4">
         <v>2052.84</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="4">
         <v>1673.68</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="4">
         <v>379.15000000000003</v>
       </c>
       <c r="F46" s="3"/>
@@ -1300,13 +1347,13 @@
       <c r="B47" s="2">
         <v>49</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="4">
         <v>15189.33</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="4">
         <v>10538.94</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="4">
         <v>4650.38</v>
       </c>
       <c r="F47" s="3"/>
@@ -1320,13 +1367,13 @@
       <c r="B48" s="2">
         <v>50</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="4">
         <v>4258.1099999999997</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="4">
         <v>3242.57</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="4">
         <v>1015.53</v>
       </c>
       <c r="F48" s="3"/>
@@ -1340,13 +1387,13 @@
       <c r="B49" s="2">
         <v>51</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="4">
         <v>39547.040000000001</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="4">
         <v>28028.47</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="4">
         <v>11518.57</v>
       </c>
       <c r="F49" s="3"/>
@@ -1360,13 +1407,13 @@
       <c r="B50" s="2">
         <v>52</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="4">
         <v>2611.59</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="4">
         <v>1881.32</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="4">
         <v>730.26</v>
       </c>
       <c r="F50" s="3"/>
@@ -1380,13 +1427,13 @@
       <c r="B51" s="2">
         <v>56</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="4">
         <v>12916.470000000001</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="4">
         <v>8748.7000000000007</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="4">
         <v>4167.7700000000004</v>
       </c>
       <c r="F51" s="3"/>
@@ -1400,13 +1447,13 @@
       <c r="B52" s="2">
         <v>57</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="4">
         <v>179.67000000000002</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="4">
         <v>164.29</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="4">
         <v>15.370000000000001</v>
       </c>
       <c r="F52" s="3"/>
@@ -1420,13 +1467,13 @@
       <c r="B53" s="2">
         <v>58</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="4">
         <v>1706.41</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="4">
         <v>1339.67</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="4">
         <v>366.74</v>
       </c>
       <c r="F53" s="3"/>
@@ -1440,13 +1487,13 @@
       <c r="B54" s="2">
         <v>61</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="4">
         <v>8170.2</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="4">
         <v>6781.6900000000005</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="4">
         <v>1388.5</v>
       </c>
       <c r="F54" s="3"/>
@@ -1460,13 +1507,13 @@
       <c r="B55" s="2">
         <v>63</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="4">
         <v>239.42000000000002</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="4">
         <v>187.59</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="4">
         <v>51.83</v>
       </c>
       <c r="F55" s="3"/>
@@ -1480,13 +1527,13 @@
       <c r="B56" s="2">
         <v>65</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="4">
         <v>4616.45</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="4">
         <v>3742.64</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="4">
         <v>873.80000000000007</v>
       </c>
       <c r="F56" s="3"/>
@@ -1500,13 +1547,13 @@
       <c r="B57" s="2">
         <v>66</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="4">
         <v>212.79</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="4">
         <v>155.76</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="4">
         <v>57.02</v>
       </c>
       <c r="F57" s="3"/>
@@ -1520,13 +1567,13 @@
       <c r="B58" s="2">
         <v>67</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="4">
         <v>86.53</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="4">
         <v>60.09</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="4">
         <v>26.42</v>
       </c>
       <c r="F58" s="3"/>
@@ -1540,13 +1587,13 @@
       <c r="B59" s="2">
         <v>68</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="4">
         <v>7953.6</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="4">
         <v>6430.95</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="4">
         <v>1522.64</v>
       </c>
       <c r="F59" s="3"/>
@@ -1560,13 +1607,13 @@
       <c r="B60" s="2">
         <v>69</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="4">
         <v>536.83000000000004</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="4">
         <v>455.27</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="4">
         <v>81.56</v>
       </c>
       <c r="F60" s="3"/>
@@ -1580,13 +1627,13 @@
       <c r="B61" s="2">
         <v>70</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="4">
         <v>18610.34</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="4">
         <v>12738.66</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="4">
         <v>5871.67</v>
       </c>
       <c r="F61" s="3"/>
@@ -1600,13 +1647,13 @@
       <c r="B62" s="2">
         <v>72</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="4">
         <v>1595.23</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="4">
         <v>1358.28</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="4">
         <v>236.94</v>
       </c>
       <c r="F62" s="3"/>
@@ -1620,13 +1667,13 @@
       <c r="B63" s="2">
         <v>73</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="4">
         <v>37372.480000000003</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="4">
         <v>30335.91</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="4">
         <v>7036.56</v>
       </c>
       <c r="F63" s="3"/>
@@ -1640,13 +1687,13 @@
       <c r="B64" s="2">
         <v>75</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="4">
         <v>16236.24</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="4">
         <v>11178.5</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="4">
         <v>5057.7300000000005</v>
       </c>
       <c r="F64" s="3"/>
@@ -1660,13 +1707,13 @@
       <c r="B65" s="2">
         <v>76</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="4">
         <v>2032.24</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="4">
         <v>1667.95</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="4">
         <v>364.29</v>
       </c>
       <c r="F65" s="3"/>
@@ -1680,13 +1727,13 @@
       <c r="B66" s="2">
         <v>77</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="4">
         <v>16884.07</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="4">
         <v>11428.74</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="4">
         <v>5455.32</v>
       </c>
       <c r="F66" s="3"/>
@@ -1700,13 +1747,13 @@
       <c r="B67" s="2">
         <v>78</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="4">
         <v>25648.880000000001</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="4">
         <v>18840.66</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="4">
         <v>6808.22</v>
       </c>
       <c r="F67" s="3"/>
@@ -1720,13 +1767,13 @@
       <c r="B68" s="2">
         <v>81</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="4">
         <v>0.43</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="4">
         <v>0.39</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="4">
         <v>0.03</v>
       </c>
       <c r="F68" s="3"/>
@@ -1740,13 +1787,13 @@
       <c r="B69" s="2">
         <v>82</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="4">
         <v>9312.2900000000009</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="4">
         <v>7608.66</v>
       </c>
-      <c r="E69" s="3">
+      <c r="E69" s="4">
         <v>1703.63</v>
       </c>
       <c r="F69" s="3"/>
@@ -1760,13 +1807,13 @@
       <c r="B70" s="2">
         <v>83</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="4">
         <v>233.09</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="4">
         <v>208.25</v>
       </c>
-      <c r="E70" s="3">
+      <c r="E70" s="4">
         <v>24.830000000000002</v>
       </c>
       <c r="F70" s="3"/>
@@ -1780,13 +1827,13 @@
       <c r="B71" s="2">
         <v>84</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="4">
         <v>4877.97</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="4">
         <v>4088.4100000000003</v>
       </c>
-      <c r="E71" s="3">
+      <c r="E71" s="4">
         <v>789.55000000000007</v>
       </c>
       <c r="F71" s="3"/>
@@ -1800,13 +1847,13 @@
       <c r="B72" s="2">
         <v>85</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="4">
         <v>331.56</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="4">
         <v>267.72000000000003</v>
       </c>
-      <c r="E72" s="3">
+      <c r="E72" s="4">
         <v>63.84</v>
       </c>
       <c r="F72" s="3"/>
@@ -1820,13 +1867,13 @@
       <c r="B73" s="2">
         <v>86</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="4">
         <v>900.87</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="4">
         <v>783.54</v>
       </c>
-      <c r="E73" s="3">
+      <c r="E73" s="4">
         <v>117.32000000000001</v>
       </c>
       <c r="F73" s="3"/>
@@ -1840,13 +1887,13 @@
       <c r="B74" s="2">
         <v>87</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="4">
         <v>14887.5</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="4">
         <v>10826.06</v>
       </c>
-      <c r="E74" s="3">
+      <c r="E74" s="4">
         <v>4061.44</v>
       </c>
       <c r="F74" s="3"/>
@@ -1860,13 +1907,13 @@
       <c r="B75" s="2">
         <v>88</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="4">
         <v>8344.7000000000007</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="4">
         <v>5594.74</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E75" s="4">
         <v>2749.9500000000003</v>
       </c>
       <c r="F75" s="3"/>
@@ -1880,13 +1927,13 @@
       <c r="B76" s="2">
         <v>89</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="4">
         <v>7134.8</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="4">
         <v>5726.61</v>
       </c>
-      <c r="E76" s="3">
+      <c r="E76" s="4">
         <v>1408.19</v>
       </c>
       <c r="F76" s="3"/>
@@ -1900,13 +1947,13 @@
       <c r="B77" s="2">
         <v>90</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="4">
         <v>16846.900000000001</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="4">
         <v>12551.470000000001</v>
       </c>
-      <c r="E77" s="3">
+      <c r="E77" s="4">
         <v>4295.42</v>
       </c>
       <c r="F77" s="3"/>
@@ -1920,13 +1967,13 @@
       <c r="B78" s="2">
         <v>91</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="4">
         <v>6869.28</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D78" s="4">
         <v>5928.37</v>
       </c>
-      <c r="E78" s="3">
+      <c r="E78" s="4">
         <v>940.91</v>
       </c>
       <c r="F78" s="3"/>
@@ -1940,13 +1987,13 @@
       <c r="B79" s="2">
         <v>93</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="4">
         <v>16940.580000000002</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D79" s="4">
         <v>10411.550000000001</v>
       </c>
-      <c r="E79" s="3">
+      <c r="E79" s="4">
         <v>6529.03</v>
       </c>
       <c r="F79" s="3"/>
@@ -1960,13 +2007,13 @@
       <c r="B80" s="2">
         <v>94</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="4">
         <v>65466.6</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="4">
         <v>51119.15</v>
       </c>
-      <c r="E80" s="3">
+      <c r="E80" s="4">
         <v>14347.44</v>
       </c>
       <c r="F80" s="3"/>
@@ -1980,13 +2027,13 @@
       <c r="B81" s="2">
         <v>96</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="4">
         <v>4309.3900000000003</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="4">
         <v>3429.46</v>
       </c>
-      <c r="E81" s="3">
+      <c r="E81" s="4">
         <v>879.93000000000006</v>
       </c>
       <c r="F81" s="3"/>
@@ -2000,13 +2047,13 @@
       <c r="B82" s="2">
         <v>97</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="4">
         <v>62.35</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="4">
         <v>37.480000000000004</v>
       </c>
-      <c r="E82" s="3">
+      <c r="E82" s="4">
         <v>24.87</v>
       </c>
       <c r="F82" s="3"/>
@@ -2020,13 +2067,13 @@
       <c r="B83" s="2">
         <v>98</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="4">
         <v>21398.45</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D83" s="4">
         <v>15623.39</v>
       </c>
-      <c r="E83" s="3">
+      <c r="E83" s="4">
         <v>5775.05</v>
       </c>
       <c r="F83" s="3"/>
@@ -2040,13 +2087,13 @@
       <c r="B84" s="2">
         <v>100</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="4">
         <v>8985.7000000000007</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="4">
         <v>6610.02</v>
       </c>
-      <c r="E84" s="3">
+      <c r="E84" s="4">
         <v>2375.66</v>
       </c>
       <c r="F84" s="3"/>
@@ -2060,13 +2107,13 @@
       <c r="B85" s="2">
         <v>101</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="4">
         <v>2322.81</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D85" s="4">
         <v>1872.3600000000001</v>
       </c>
-      <c r="E85" s="3">
+      <c r="E85" s="4">
         <v>450.44</v>
       </c>
       <c r="F85" s="3"/>
@@ -2080,13 +2127,13 @@
       <c r="B86" s="2">
         <v>102</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="4">
         <v>2061.77</v>
       </c>
-      <c r="D86" s="3">
+      <c r="D86" s="4">
         <v>1457.39</v>
       </c>
-      <c r="E86" s="3">
+      <c r="E86" s="4">
         <v>604.38</v>
       </c>
       <c r="F86" s="3"/>
@@ -2100,13 +2147,13 @@
       <c r="B87" s="2">
         <v>103</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="4">
         <v>68076.36</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D87" s="4">
         <v>48097.32</v>
       </c>
-      <c r="E87" s="3">
+      <c r="E87" s="4">
         <v>19979.03</v>
       </c>
       <c r="F87" s="3"/>
@@ -2120,13 +2167,13 @@
       <c r="B88" s="2">
         <v>107</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="4">
         <v>5202.3599999999997</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D88" s="4">
         <v>4675.8599999999997</v>
       </c>
-      <c r="E88" s="3">
+      <c r="E88" s="4">
         <v>526.49</v>
       </c>
       <c r="F88" s="3"/>
@@ -2140,13 +2187,13 @@
       <c r="B89" s="2">
         <v>109</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="4">
         <v>29355.72</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D89" s="4">
         <v>23166.560000000001</v>
       </c>
-      <c r="E89" s="3">
+      <c r="E89" s="4">
         <v>6189.1500000000005</v>
       </c>
       <c r="F89" s="3"/>
@@ -2160,13 +2207,13 @@
       <c r="B90" s="2">
         <v>110</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="4">
         <v>1143.3</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="4">
         <v>927.73</v>
       </c>
-      <c r="E90" s="3">
+      <c r="E90" s="4">
         <v>215.55</v>
       </c>
       <c r="F90" s="3"/>
@@ -2180,13 +2227,13 @@
       <c r="B91" s="2">
         <v>111</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="4">
         <v>3853.77</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D91" s="4">
         <v>2785.2200000000003</v>
       </c>
-      <c r="E91" s="3">
+      <c r="E91" s="4">
         <v>1068.54</v>
       </c>
       <c r="F91" s="3"/>
@@ -2200,13 +2247,13 @@
       <c r="B92" s="2">
         <v>112</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92" s="4">
         <v>62898.83</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D92" s="4">
         <v>48853.120000000003</v>
       </c>
-      <c r="E92" s="3">
+      <c r="E92" s="4">
         <v>14045.7</v>
       </c>
       <c r="F92" s="3"/>
@@ -2220,13 +2267,13 @@
       <c r="B93" s="2">
         <v>113</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93" s="4">
         <v>1829.29</v>
       </c>
-      <c r="D93" s="3">
+      <c r="D93" s="4">
         <v>1244.07</v>
       </c>
-      <c r="E93" s="3">
+      <c r="E93" s="4">
         <v>585.21</v>
       </c>
       <c r="F93" s="3"/>
@@ -2240,13 +2287,13 @@
       <c r="B94" s="2">
         <v>114</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94" s="4">
         <v>8080.6100000000006</v>
       </c>
-      <c r="D94" s="3">
+      <c r="D94" s="4">
         <v>6554.67</v>
       </c>
-      <c r="E94" s="3">
+      <c r="E94" s="4">
         <v>1525.93</v>
       </c>
       <c r="F94" s="3"/>
@@ -2260,13 +2307,13 @@
       <c r="B95" s="2">
         <v>115</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95" s="4">
         <v>20894.91</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D95" s="4">
         <v>16540.28</v>
       </c>
-      <c r="E95" s="3">
+      <c r="E95" s="4">
         <v>4354.62</v>
       </c>
       <c r="F95" s="3"/>
@@ -2280,13 +2327,13 @@
       <c r="B96" s="2">
         <v>116</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96" s="4">
         <v>27165.05</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="4">
         <v>22396.79</v>
       </c>
-      <c r="E96" s="3">
+      <c r="E96" s="4">
         <v>4768.26</v>
       </c>
       <c r="F96" s="3"/>
@@ -2300,13 +2347,13 @@
       <c r="B97" s="2">
         <v>117</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97" s="4">
         <v>26027.850000000002</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="4">
         <v>14334.74</v>
       </c>
-      <c r="E97" s="3">
+      <c r="E97" s="4">
         <v>11693.04</v>
       </c>
       <c r="F97" s="3"/>
@@ -2320,13 +2367,13 @@
       <c r="B98" s="2">
         <v>119</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="4">
         <v>1362.55</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D98" s="4">
         <v>1046.1200000000001</v>
       </c>
-      <c r="E98" s="3">
+      <c r="E98" s="4">
         <v>316.43</v>
       </c>
       <c r="F98" s="3"/>
@@ -2340,13 +2387,13 @@
       <c r="B99" s="2">
         <v>120</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="4">
         <v>4.8</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="4">
         <v>4.8</v>
       </c>
-      <c r="E99" s="3">
+      <c r="E99" s="4">
         <v>0</v>
       </c>
       <c r="F99" s="3"/>
@@ -2360,13 +2407,13 @@
       <c r="B100" s="2">
         <v>121</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="4">
         <v>6889</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D100" s="4">
         <v>5065.9800000000005</v>
       </c>
-      <c r="E100" s="3">
+      <c r="E100" s="4">
         <v>1823.02</v>
       </c>
       <c r="F100" s="3"/>
@@ -2380,13 +2427,13 @@
       <c r="B101" s="2">
         <v>122</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="4">
         <v>10655.86</v>
       </c>
-      <c r="D101" s="3">
+      <c r="D101" s="4">
         <v>5392.96</v>
       </c>
-      <c r="E101" s="3">
+      <c r="E101" s="4">
         <v>5262.9000000000005</v>
       </c>
       <c r="F101" s="3"/>
@@ -2400,13 +2447,13 @@
       <c r="B102" s="2">
         <v>123</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="4">
         <v>5246.47</v>
       </c>
-      <c r="D102" s="3">
+      <c r="D102" s="4">
         <v>3840.4</v>
       </c>
-      <c r="E102" s="3">
+      <c r="E102" s="4">
         <v>1406.06</v>
       </c>
       <c r="F102" s="3"/>
@@ -2420,13 +2467,13 @@
       <c r="B103" s="2">
         <v>124</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="4">
         <v>16058.68</v>
       </c>
-      <c r="D103" s="3">
+      <c r="D103" s="4">
         <v>11803.24</v>
       </c>
-      <c r="E103" s="3">
+      <c r="E103" s="4">
         <v>4255.43</v>
       </c>
       <c r="F103" s="3"/>
@@ -2440,13 +2487,13 @@
       <c r="B104" s="2">
         <v>125</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C104" s="4">
         <v>5803.5</v>
       </c>
-      <c r="D104" s="3">
+      <c r="D104" s="4">
         <v>4612.93</v>
       </c>
-      <c r="E104" s="3">
+      <c r="E104" s="4">
         <v>1190.56</v>
       </c>
       <c r="F104" s="3"/>
@@ -2460,13 +2507,13 @@
       <c r="B105" s="2">
         <v>126</v>
       </c>
-      <c r="C105" s="3">
+      <c r="C105" s="4">
         <v>13872.62</v>
       </c>
-      <c r="D105" s="3">
+      <c r="D105" s="4">
         <v>10432.77</v>
       </c>
-      <c r="E105" s="3">
+      <c r="E105" s="4">
         <v>3439.84</v>
       </c>
       <c r="F105" s="3"/>
@@ -2480,13 +2527,13 @@
       <c r="B106" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C106" s="4">
         <v>118.10000000000001</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D106" s="4">
         <v>117.02</v>
       </c>
-      <c r="E106" s="3">
+      <c r="E106" s="4">
         <v>1.07</v>
       </c>
       <c r="F106" s="3"/>
@@ -2500,13 +2547,13 @@
       <c r="B107" s="2">
         <v>131</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C107" s="4">
         <v>0.63</v>
       </c>
-      <c r="D107" s="3">
+      <c r="D107" s="4">
         <v>0.47000000000000003</v>
       </c>
-      <c r="E107" s="3">
+      <c r="E107" s="4">
         <v>0.16</v>
       </c>
       <c r="F107" s="3"/>
@@ -2520,13 +2567,13 @@
       <c r="B108" s="2">
         <v>132</v>
       </c>
-      <c r="C108" s="3">
+      <c r="C108" s="4">
         <v>907.55000000000007</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="4">
         <v>714.61</v>
       </c>
-      <c r="E108" s="3">
+      <c r="E108" s="4">
         <v>192.94</v>
       </c>
       <c r="F108" s="3"/>
@@ -2534,7 +2581,7 @@
       <c r="H108" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A1:H113">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H113">
     <sortCondition ref="F1:F113"/>
   </sortState>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.59055118110236227" bottom="0.84051968503937013" header="0.59055118110236227" footer="0.59055118110236227"/>

</xml_diff>